<commit_message>
add repositories, service, improve code
</commit_message>
<xml_diff>
--- a/src/main/resources/ReactorData.xlsx
+++ b/src/main/resources/ReactorData.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="192" yWindow="72" windowWidth="20100" windowHeight="5856"/>
@@ -14,14 +14,14 @@
     <sheet name="companies" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">units!$A$1:$S$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">units!$A$1:$S$625</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4797" uniqueCount="1996">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4797" uniqueCount="1998">
   <si>
     <t>id</t>
   </si>
@@ -6009,6 +6009,12 @@
   </si>
   <si>
     <t>Bangladesh 	Atomic Energy Commissio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stoped                                                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">stoped                                                                    </t>
   </si>
 </sst>
 </file>
@@ -6016,7 +6022,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="dd\-mmm\-yy"/>
+    <numFmt numFmtId="164" formatCode="dd\-mmm\-yy"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -6142,7 +6148,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -6495,7 +6501,7 @@
   <dimension ref="A1:S625"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1"/>
+      <selection activeCell="H52" sqref="H52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6947,7 +6953,7 @@
         <v>56</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>21</v>
+        <v>1996</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>33</v>
@@ -7051,7 +7057,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -7110,7 +7116,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -7169,7 +7175,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -7873,7 +7879,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -7991,7 +7997,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -8109,7 +8115,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="28" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -8168,7 +8174,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -8522,7 +8528,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -8581,7 +8587,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -8699,7 +8705,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="38" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -8758,7 +8764,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="39" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -8817,7 +8823,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="40" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -9157,7 +9163,7 @@
       </c>
       <c r="S45" s="5"/>
     </row>
-    <row r="46" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -9216,7 +9222,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="47" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -9275,7 +9281,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="48" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -9334,7 +9340,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="49" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -9393,7 +9399,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="50" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -9448,7 +9454,7 @@
       </c>
       <c r="S50" s="5"/>
     </row>
-    <row r="51" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -9503,7 +9509,7 @@
       </c>
       <c r="S51" s="5"/>
     </row>
-    <row r="52" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -9558,7 +9564,7 @@
       </c>
       <c r="S52" s="5"/>
     </row>
-    <row r="53" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -9731,7 +9737,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="56" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -9790,7 +9796,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="57" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -9849,7 +9855,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="58" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -9908,7 +9914,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="59" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -10191,7 +10197,7 @@
       </c>
       <c r="S63" s="5"/>
     </row>
-    <row r="64" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
         <v>63</v>
       </c>
@@ -10246,7 +10252,7 @@
       </c>
       <c r="S64" s="5"/>
     </row>
-    <row r="65" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
         <v>64</v>
       </c>
@@ -11673,7 +11679,7 @@
       </c>
       <c r="S89" s="5"/>
     </row>
-    <row r="90" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A90" s="2">
         <v>89</v>
       </c>
@@ -11732,7 +11738,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="91" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A91" s="2">
         <v>90</v>
       </c>
@@ -11791,7 +11797,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="92" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A92" s="2">
         <v>91</v>
       </c>
@@ -11850,7 +11856,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="93" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A93" s="2">
         <v>92</v>
       </c>
@@ -11909,7 +11915,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="94" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A94" s="2">
         <v>93</v>
       </c>
@@ -12082,7 +12088,7 @@
       </c>
       <c r="S96" s="5"/>
     </row>
-    <row r="97" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A97" s="2">
         <v>96</v>
       </c>
@@ -12139,7 +12145,7 @@
       </c>
       <c r="S97" s="5"/>
     </row>
-    <row r="98" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A98" s="2">
         <v>97</v>
       </c>
@@ -12196,7 +12202,7 @@
       </c>
       <c r="S98" s="5"/>
     </row>
-    <row r="99" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A99" s="2">
         <v>98</v>
       </c>
@@ -12251,7 +12257,7 @@
       </c>
       <c r="S99" s="5"/>
     </row>
-    <row r="100" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A100" s="2">
         <v>99</v>
       </c>
@@ -12933,7 +12939,7 @@
       </c>
       <c r="S111" s="5"/>
     </row>
-    <row r="112" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A112" s="2">
         <v>111</v>
       </c>
@@ -12988,7 +12994,7 @@
       </c>
       <c r="S112" s="5"/>
     </row>
-    <row r="113" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A113" s="2">
         <v>112</v>
       </c>
@@ -13491,7 +13497,7 @@
       </c>
       <c r="S121" s="5"/>
     </row>
-    <row r="122" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A122" s="2">
         <v>121</v>
       </c>
@@ -13550,7 +13556,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="123" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A123" s="2">
         <v>122</v>
       </c>
@@ -13609,7 +13615,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="124" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A124" s="2">
         <v>123</v>
       </c>
@@ -13668,7 +13674,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="125" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A125" s="2">
         <v>124</v>
       </c>
@@ -13845,7 +13851,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="128" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A128" s="2">
         <v>127</v>
       </c>
@@ -13902,7 +13908,7 @@
       </c>
       <c r="S128" s="5"/>
     </row>
-    <row r="129" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A129" s="2">
         <v>128</v>
       </c>
@@ -14016,7 +14022,7 @@
       </c>
       <c r="S130" s="5"/>
     </row>
-    <row r="131" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A131" s="2">
         <v>130</v>
       </c>
@@ -14073,7 +14079,7 @@
       </c>
       <c r="S131" s="5"/>
     </row>
-    <row r="132" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A132" s="2">
         <v>131</v>
       </c>
@@ -14130,7 +14136,7 @@
       </c>
       <c r="S132" s="5"/>
     </row>
-    <row r="133" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A133" s="2">
         <v>132</v>
       </c>
@@ -14185,7 +14191,7 @@
       </c>
       <c r="S133" s="5"/>
     </row>
-    <row r="134" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A134" s="2">
         <v>133</v>
       </c>
@@ -14684,7 +14690,7 @@
       </c>
       <c r="S142" s="5"/>
     </row>
-    <row r="143" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A143" s="2">
         <v>142</v>
       </c>
@@ -14739,7 +14745,7 @@
       </c>
       <c r="S143" s="5"/>
     </row>
-    <row r="144" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A144" s="2">
         <v>143</v>
       </c>
@@ -14794,7 +14800,7 @@
       </c>
       <c r="S144" s="5"/>
     </row>
-    <row r="145" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A145" s="2">
         <v>144</v>
       </c>
@@ -14849,7 +14855,7 @@
       </c>
       <c r="S145" s="5"/>
     </row>
-    <row r="146" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A146" s="2">
         <v>145</v>
       </c>
@@ -14904,7 +14910,7 @@
       </c>
       <c r="S146" s="5"/>
     </row>
-    <row r="147" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A147" s="2">
         <v>146</v>
       </c>
@@ -14959,7 +14965,7 @@
       </c>
       <c r="S147" s="5"/>
     </row>
-    <row r="148" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A148" s="2">
         <v>147</v>
       </c>
@@ -15014,7 +15020,7 @@
       </c>
       <c r="S148" s="5"/>
     </row>
-    <row r="149" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A149" s="2">
         <v>148</v>
       </c>
@@ -15069,7 +15075,7 @@
       </c>
       <c r="S149" s="5"/>
     </row>
-    <row r="150" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A150" s="2">
         <v>149</v>
       </c>
@@ -15124,7 +15130,7 @@
       </c>
       <c r="S150" s="5"/>
     </row>
-    <row r="151" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A151" s="2">
         <v>150</v>
       </c>
@@ -15179,7 +15185,7 @@
       </c>
       <c r="S151" s="5"/>
     </row>
-    <row r="152" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A152" s="2">
         <v>151</v>
       </c>
@@ -15234,7 +15240,7 @@
       </c>
       <c r="S152" s="5"/>
     </row>
-    <row r="153" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A153" s="2">
         <v>152</v>
       </c>
@@ -15289,7 +15295,7 @@
       </c>
       <c r="S153" s="5"/>
     </row>
-    <row r="154" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A154" s="2">
         <v>153</v>
       </c>
@@ -15564,7 +15570,7 @@
       </c>
       <c r="S158" s="5"/>
     </row>
-    <row r="159" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A159" s="2">
         <v>158</v>
       </c>
@@ -15619,7 +15625,7 @@
       </c>
       <c r="S159" s="5"/>
     </row>
-    <row r="160" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A160" s="2">
         <v>159</v>
       </c>
@@ -15674,7 +15680,7 @@
       </c>
       <c r="S160" s="5"/>
     </row>
-    <row r="161" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A161" s="2">
         <v>160</v>
       </c>
@@ -15729,7 +15735,7 @@
       </c>
       <c r="S161" s="5"/>
     </row>
-    <row r="162" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A162" s="2">
         <v>161</v>
       </c>
@@ -16059,7 +16065,7 @@
       </c>
       <c r="S167" s="5"/>
     </row>
-    <row r="168" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A168" s="2">
         <v>167</v>
       </c>
@@ -16114,7 +16120,7 @@
       </c>
       <c r="S168" s="5"/>
     </row>
-    <row r="169" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A169" s="2">
         <v>168</v>
       </c>
@@ -16499,7 +16505,7 @@
       </c>
       <c r="S175" s="5"/>
     </row>
-    <row r="176" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A176" s="2">
         <v>175</v>
       </c>
@@ -16554,7 +16560,7 @@
       </c>
       <c r="S176" s="5"/>
     </row>
-    <row r="177" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A177" s="2">
         <v>176</v>
       </c>
@@ -16609,7 +16615,7 @@
       </c>
       <c r="S177" s="5"/>
     </row>
-    <row r="178" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A178" s="2">
         <v>177</v>
       </c>
@@ -16664,7 +16670,7 @@
       </c>
       <c r="S178" s="5"/>
     </row>
-    <row r="179" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A179" s="2">
         <v>178</v>
       </c>
@@ -16719,7 +16725,7 @@
       </c>
       <c r="S179" s="5"/>
     </row>
-    <row r="180" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A180" s="2">
         <v>179</v>
       </c>
@@ -16774,7 +16780,7 @@
       </c>
       <c r="S180" s="5"/>
     </row>
-    <row r="181" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A181" s="2">
         <v>180</v>
       </c>
@@ -16829,7 +16835,7 @@
       </c>
       <c r="S181" s="5"/>
     </row>
-    <row r="182" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A182" s="2">
         <v>181</v>
       </c>
@@ -16884,7 +16890,7 @@
       </c>
       <c r="S182" s="5"/>
     </row>
-    <row r="183" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A183" s="2">
         <v>182</v>
       </c>
@@ -16939,7 +16945,7 @@
       </c>
       <c r="S183" s="5"/>
     </row>
-    <row r="184" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A184" s="2">
         <v>183</v>
       </c>
@@ -16994,7 +17000,7 @@
       </c>
       <c r="S184" s="5"/>
     </row>
-    <row r="185" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A185" s="2">
         <v>184</v>
       </c>
@@ -17049,7 +17055,7 @@
       </c>
       <c r="S185" s="5"/>
     </row>
-    <row r="186" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A186" s="2">
         <v>185</v>
       </c>
@@ -17104,7 +17110,7 @@
       </c>
       <c r="S186" s="5"/>
     </row>
-    <row r="187" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A187" s="2">
         <v>186</v>
       </c>
@@ -17159,7 +17165,7 @@
       </c>
       <c r="S187" s="5"/>
     </row>
-    <row r="188" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A188" s="2">
         <v>187</v>
       </c>
@@ -17214,7 +17220,7 @@
       </c>
       <c r="S188" s="5"/>
     </row>
-    <row r="189" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A189" s="2">
         <v>188</v>
       </c>
@@ -17269,7 +17275,7 @@
       </c>
       <c r="S189" s="5"/>
     </row>
-    <row r="190" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A190" s="2">
         <v>189</v>
       </c>
@@ -17324,7 +17330,7 @@
       </c>
       <c r="S190" s="5"/>
     </row>
-    <row r="191" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A191" s="2">
         <v>190</v>
       </c>
@@ -17393,7 +17399,7 @@
         <v>23</v>
       </c>
       <c r="E192" s="3" t="s">
-        <v>21</v>
+        <v>1997</v>
       </c>
       <c r="F192" s="3" t="s">
         <v>33</v>
@@ -17452,7 +17458,7 @@
         <v>63</v>
       </c>
       <c r="E193" s="3" t="s">
-        <v>21</v>
+        <v>1997</v>
       </c>
       <c r="F193" s="3" t="s">
         <v>33</v>
@@ -17497,7 +17503,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="194" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A194" s="2">
         <v>193</v>
       </c>
@@ -17568,7 +17574,7 @@
         <v>81</v>
       </c>
       <c r="E195" s="3" t="s">
-        <v>21</v>
+        <v>1997</v>
       </c>
       <c r="F195" s="3" t="s">
         <v>33</v>
@@ -17627,7 +17633,7 @@
         <v>140</v>
       </c>
       <c r="E196" s="3" t="s">
-        <v>21</v>
+        <v>1997</v>
       </c>
       <c r="F196" s="3" t="s">
         <v>33</v>
@@ -17672,7 +17678,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="197" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A197" s="2">
         <v>196</v>
       </c>
@@ -17686,7 +17692,7 @@
         <v>165</v>
       </c>
       <c r="E197" s="3" t="s">
-        <v>21</v>
+        <v>1997</v>
       </c>
       <c r="F197" s="3" t="s">
         <v>33</v>
@@ -17731,7 +17737,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="198" spans="1:19" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A198" s="2">
         <v>197</v>
       </c>
@@ -17745,7 +17751,7 @@
         <v>83</v>
       </c>
       <c r="E198" s="3" t="s">
-        <v>21</v>
+        <v>1997</v>
       </c>
       <c r="F198" s="3" t="s">
         <v>323</v>
@@ -17790,7 +17796,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="199" spans="1:19" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A199" s="2">
         <v>198</v>
       </c>
@@ -17847,7 +17853,7 @@
       </c>
       <c r="S199" s="5"/>
     </row>
-    <row r="200" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A200" s="2">
         <v>199</v>
       </c>
@@ -17861,7 +17867,7 @@
         <v>102</v>
       </c>
       <c r="E200" s="3" t="s">
-        <v>21</v>
+        <v>1997</v>
       </c>
       <c r="F200" s="3" t="s">
         <v>33</v>
@@ -17906,7 +17912,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="201" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A201" s="2">
         <v>200</v>
       </c>
@@ -17963,7 +17969,7 @@
       </c>
       <c r="S201" s="5"/>
     </row>
-    <row r="202" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A202" s="2">
         <v>201</v>
       </c>
@@ -18020,7 +18026,7 @@
       </c>
       <c r="S202" s="5"/>
     </row>
-    <row r="203" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A203" s="2">
         <v>202</v>
       </c>
@@ -18077,7 +18083,7 @@
       </c>
       <c r="S203" s="5"/>
     </row>
-    <row r="204" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A204" s="2">
         <v>203</v>
       </c>
@@ -18354,7 +18360,7 @@
       </c>
       <c r="S208" s="5"/>
     </row>
-    <row r="209" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A209" s="2">
         <v>208</v>
       </c>
@@ -18409,7 +18415,7 @@
       </c>
       <c r="S209" s="5"/>
     </row>
-    <row r="210" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A210" s="2">
         <v>209</v>
       </c>
@@ -18680,7 +18686,7 @@
       </c>
       <c r="S214" s="5"/>
     </row>
-    <row r="215" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A215" s="2">
         <v>214</v>
       </c>
@@ -18735,7 +18741,7 @@
       </c>
       <c r="S215" s="5"/>
     </row>
-    <row r="216" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A216" s="2">
         <v>215</v>
       </c>
@@ -18790,7 +18796,7 @@
       </c>
       <c r="S216" s="5"/>
     </row>
-    <row r="217" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A217" s="2">
         <v>216</v>
       </c>
@@ -18845,7 +18851,7 @@
       </c>
       <c r="S217" s="5"/>
     </row>
-    <row r="218" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A218" s="2">
         <v>217</v>
       </c>
@@ -18953,7 +18959,7 @@
       </c>
       <c r="S219" s="5"/>
     </row>
-    <row r="220" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A220" s="2">
         <v>219</v>
       </c>
@@ -19008,7 +19014,7 @@
       </c>
       <c r="S220" s="5"/>
     </row>
-    <row r="221" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A221" s="2">
         <v>220</v>
       </c>
@@ -19063,7 +19069,7 @@
       </c>
       <c r="S221" s="5"/>
     </row>
-    <row r="222" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A222" s="2">
         <v>221</v>
       </c>
@@ -19118,7 +19124,7 @@
       </c>
       <c r="S222" s="5"/>
     </row>
-    <row r="223" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A223" s="2">
         <v>222</v>
       </c>
@@ -19173,7 +19179,7 @@
       </c>
       <c r="S223" s="5"/>
     </row>
-    <row r="224" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A224" s="2">
         <v>223</v>
       </c>
@@ -19228,7 +19234,7 @@
       </c>
       <c r="S224" s="5"/>
     </row>
-    <row r="225" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A225" s="2">
         <v>224</v>
       </c>
@@ -19393,7 +19399,7 @@
       </c>
       <c r="S227" s="5"/>
     </row>
-    <row r="228" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A228" s="2">
         <v>227</v>
       </c>
@@ -19448,7 +19454,7 @@
       </c>
       <c r="S228" s="5"/>
     </row>
-    <row r="229" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A229" s="2">
         <v>228</v>
       </c>
@@ -19503,7 +19509,7 @@
       </c>
       <c r="S229" s="5"/>
     </row>
-    <row r="230" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A230" s="2">
         <v>229</v>
       </c>
@@ -19558,7 +19564,7 @@
       </c>
       <c r="S230" s="5"/>
     </row>
-    <row r="231" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A231" s="2">
         <v>230</v>
       </c>
@@ -19668,7 +19674,7 @@
       </c>
       <c r="S232" s="5"/>
     </row>
-    <row r="233" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A233" s="2">
         <v>232</v>
       </c>
@@ -19719,7 +19725,7 @@
       </c>
       <c r="S233" s="5"/>
     </row>
-    <row r="234" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A234" s="2">
         <v>233</v>
       </c>
@@ -19770,7 +19776,7 @@
       </c>
       <c r="S234" s="5"/>
     </row>
-    <row r="235" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A235" s="2">
         <v>234</v>
       </c>
@@ -19821,7 +19827,7 @@
       </c>
       <c r="S235" s="5"/>
     </row>
-    <row r="236" spans="1:19" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A236" s="2">
         <v>235</v>
       </c>
@@ -19876,7 +19882,7 @@
       </c>
       <c r="S236" s="5"/>
     </row>
-    <row r="237" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A237" s="2">
         <v>236</v>
       </c>
@@ -19931,7 +19937,7 @@
       </c>
       <c r="S237" s="5"/>
     </row>
-    <row r="238" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A238" s="2">
         <v>237</v>
       </c>
@@ -19986,7 +19992,7 @@
       </c>
       <c r="S238" s="5"/>
     </row>
-    <row r="239" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A239" s="2">
         <v>238</v>
       </c>
@@ -20041,7 +20047,7 @@
       </c>
       <c r="S239" s="5"/>
     </row>
-    <row r="240" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A240" s="2">
         <v>239</v>
       </c>
@@ -20096,7 +20102,7 @@
       </c>
       <c r="S240" s="5"/>
     </row>
-    <row r="241" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A241" s="2">
         <v>240</v>
       </c>
@@ -20206,7 +20212,7 @@
       </c>
       <c r="S242" s="5"/>
     </row>
-    <row r="243" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A243" s="2">
         <v>242</v>
       </c>
@@ -20261,7 +20267,7 @@
       </c>
       <c r="S243" s="5"/>
     </row>
-    <row r="244" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A244" s="2">
         <v>243</v>
       </c>
@@ -20536,7 +20542,7 @@
       </c>
       <c r="S248" s="5"/>
     </row>
-    <row r="249" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A249" s="2">
         <v>248</v>
       </c>
@@ -20591,7 +20597,7 @@
       </c>
       <c r="S249" s="5"/>
     </row>
-    <row r="250" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A250" s="2">
         <v>249</v>
       </c>
@@ -20646,7 +20652,7 @@
       </c>
       <c r="S250" s="5"/>
     </row>
-    <row r="251" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A251" s="2">
         <v>250</v>
       </c>
@@ -20697,7 +20703,7 @@
       </c>
       <c r="S251" s="5"/>
     </row>
-    <row r="252" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A252" s="2">
         <v>251</v>
       </c>
@@ -20748,7 +20754,7 @@
       </c>
       <c r="S252" s="5"/>
     </row>
-    <row r="253" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A253" s="2">
         <v>252</v>
       </c>
@@ -20799,7 +20805,7 @@
       </c>
       <c r="S253" s="5"/>
     </row>
-    <row r="254" spans="1:19" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A254" s="2">
         <v>253</v>
       </c>
@@ -21113,7 +21119,7 @@
       </c>
       <c r="S259" s="5"/>
     </row>
-    <row r="260" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A260" s="2">
         <v>259</v>
       </c>
@@ -21168,7 +21174,7 @@
       </c>
       <c r="S260" s="5"/>
     </row>
-    <row r="261" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A261" s="2">
         <v>260</v>
       </c>
@@ -21223,7 +21229,7 @@
       </c>
       <c r="S261" s="5"/>
     </row>
-    <row r="262" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A262" s="2">
         <v>261</v>
       </c>
@@ -21278,7 +21284,7 @@
       </c>
       <c r="S262" s="5"/>
     </row>
-    <row r="263" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A263" s="2">
         <v>262</v>
       </c>
@@ -21333,7 +21339,7 @@
       </c>
       <c r="S263" s="5"/>
     </row>
-    <row r="264" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A264" s="2">
         <v>263</v>
       </c>
@@ -21388,7 +21394,7 @@
       </c>
       <c r="S264" s="5"/>
     </row>
-    <row r="265" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A265" s="2">
         <v>264</v>
       </c>
@@ -21443,7 +21449,7 @@
       </c>
       <c r="S265" s="5"/>
     </row>
-    <row r="266" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A266" s="2">
         <v>265</v>
       </c>
@@ -21771,7 +21777,7 @@
       </c>
       <c r="S271" s="5"/>
     </row>
-    <row r="272" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A272" s="2">
         <v>271</v>
       </c>
@@ -22042,7 +22048,7 @@
       </c>
       <c r="S276" s="5"/>
     </row>
-    <row r="277" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A277" s="2">
         <v>276</v>
       </c>
@@ -22150,7 +22156,7 @@
       </c>
       <c r="S278" s="5"/>
     </row>
-    <row r="279" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A279" s="2">
         <v>278</v>
       </c>
@@ -22205,7 +22211,7 @@
       </c>
       <c r="S279" s="5"/>
     </row>
-    <row r="280" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A280" s="2">
         <v>279</v>
       </c>
@@ -22260,7 +22266,7 @@
       </c>
       <c r="S280" s="5"/>
     </row>
-    <row r="281" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A281" s="2">
         <v>280</v>
       </c>
@@ -22315,7 +22321,7 @@
       </c>
       <c r="S281" s="5"/>
     </row>
-    <row r="282" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A282" s="2">
         <v>281</v>
       </c>
@@ -22535,7 +22541,7 @@
       </c>
       <c r="S285" s="5"/>
     </row>
-    <row r="286" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A286" s="2">
         <v>285</v>
       </c>
@@ -22590,7 +22596,7 @@
       </c>
       <c r="S286" s="5"/>
     </row>
-    <row r="287" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A287" s="2">
         <v>286</v>
       </c>
@@ -22641,7 +22647,7 @@
       </c>
       <c r="S287" s="5"/>
     </row>
-    <row r="288" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A288" s="2">
         <v>287</v>
       </c>
@@ -22692,7 +22698,7 @@
       </c>
       <c r="S288" s="5"/>
     </row>
-    <row r="289" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A289" s="2">
         <v>288</v>
       </c>
@@ -22747,7 +22753,7 @@
       </c>
       <c r="S289" s="5"/>
     </row>
-    <row r="290" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A290" s="2">
         <v>289</v>
       </c>
@@ -22802,7 +22808,7 @@
       </c>
       <c r="S290" s="5"/>
     </row>
-    <row r="291" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A291" s="2">
         <v>290</v>
       </c>
@@ -22857,7 +22863,7 @@
       </c>
       <c r="S291" s="5"/>
     </row>
-    <row r="292" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A292" s="2">
         <v>291</v>
       </c>
@@ -22967,7 +22973,7 @@
       </c>
       <c r="S293" s="5"/>
     </row>
-    <row r="294" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A294" s="2">
         <v>293</v>
       </c>
@@ -23022,7 +23028,7 @@
       </c>
       <c r="S294" s="5"/>
     </row>
-    <row r="295" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A295" s="2">
         <v>294</v>
       </c>
@@ -23077,7 +23083,7 @@
       </c>
       <c r="S295" s="5"/>
     </row>
-    <row r="296" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A296" s="2">
         <v>295</v>
       </c>
@@ -23179,7 +23185,7 @@
       </c>
       <c r="S297" s="5"/>
     </row>
-    <row r="298" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A298" s="2">
         <v>297</v>
       </c>
@@ -23234,7 +23240,7 @@
       </c>
       <c r="S298" s="5"/>
     </row>
-    <row r="299" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A299" s="2">
         <v>298</v>
       </c>
@@ -23289,7 +23295,7 @@
       </c>
       <c r="S299" s="5"/>
     </row>
-    <row r="300" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A300" s="2">
         <v>299</v>
       </c>
@@ -23344,7 +23350,7 @@
       </c>
       <c r="S300" s="5"/>
     </row>
-    <row r="301" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A301" s="2">
         <v>300</v>
       </c>
@@ -23399,7 +23405,7 @@
       </c>
       <c r="S301" s="5"/>
     </row>
-    <row r="302" spans="1:19" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A302" s="2">
         <v>301</v>
       </c>
@@ -23454,7 +23460,7 @@
       </c>
       <c r="S302" s="5"/>
     </row>
-    <row r="303" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A303" s="2">
         <v>302</v>
       </c>
@@ -23509,7 +23515,7 @@
       </c>
       <c r="S303" s="5"/>
     </row>
-    <row r="304" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A304" s="2">
         <v>303</v>
       </c>
@@ -23564,7 +23570,7 @@
       </c>
       <c r="S304" s="5"/>
     </row>
-    <row r="305" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A305" s="2">
         <v>304</v>
       </c>
@@ -23619,7 +23625,7 @@
       </c>
       <c r="S305" s="5"/>
     </row>
-    <row r="306" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A306" s="2">
         <v>305</v>
       </c>
@@ -24660,7 +24666,7 @@
       </c>
       <c r="S324" s="5"/>
     </row>
-    <row r="325" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A325" s="2">
         <v>324</v>
       </c>
@@ -24715,7 +24721,7 @@
       </c>
       <c r="S325" s="5"/>
     </row>
-    <row r="326" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A326" s="2">
         <v>325</v>
       </c>
@@ -24876,7 +24882,7 @@
       </c>
       <c r="S328" s="5"/>
     </row>
-    <row r="329" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A329" s="2">
         <v>328</v>
       </c>
@@ -24931,7 +24937,7 @@
       </c>
       <c r="S329" s="5"/>
     </row>
-    <row r="330" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A330" s="2">
         <v>329</v>
       </c>
@@ -25149,7 +25155,7 @@
       </c>
       <c r="S333" s="5"/>
     </row>
-    <row r="334" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A334" s="2">
         <v>333</v>
       </c>
@@ -25204,7 +25210,7 @@
       </c>
       <c r="S334" s="5"/>
     </row>
-    <row r="335" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A335" s="2">
         <v>334</v>
       </c>
@@ -26174,7 +26180,7 @@
       </c>
       <c r="S352" s="5"/>
     </row>
-    <row r="353" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A353" s="2">
         <v>352</v>
       </c>
@@ -26284,7 +26290,7 @@
       </c>
       <c r="S354" s="5"/>
     </row>
-    <row r="355" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A355" s="2">
         <v>354</v>
       </c>
@@ -26335,7 +26341,7 @@
       </c>
       <c r="S355" s="5"/>
     </row>
-    <row r="356" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A356" s="2">
         <v>355</v>
       </c>
@@ -26390,7 +26396,7 @@
       </c>
       <c r="S356" s="5"/>
     </row>
-    <row r="357" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A357" s="2">
         <v>356</v>
       </c>
@@ -26445,7 +26451,7 @@
       </c>
       <c r="S357" s="5"/>
     </row>
-    <row r="358" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A358" s="2">
         <v>357</v>
       </c>
@@ -26500,7 +26506,7 @@
       </c>
       <c r="S358" s="5"/>
     </row>
-    <row r="359" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A359" s="2">
         <v>358</v>
       </c>
@@ -26979,7 +26985,7 @@
       </c>
       <c r="S367" s="5"/>
     </row>
-    <row r="368" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A368" s="2">
         <v>367</v>
       </c>
@@ -27034,7 +27040,7 @@
       </c>
       <c r="S368" s="5"/>
     </row>
-    <row r="369" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A369" s="2">
         <v>368</v>
       </c>
@@ -27089,7 +27095,7 @@
       </c>
       <c r="S369" s="5"/>
     </row>
-    <row r="370" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A370" s="2">
         <v>369</v>
       </c>
@@ -27144,7 +27150,7 @@
       </c>
       <c r="S370" s="5"/>
     </row>
-    <row r="371" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A371" s="2">
         <v>370</v>
       </c>
@@ -27890,7 +27896,7 @@
       </c>
       <c r="S384" s="5"/>
     </row>
-    <row r="385" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A385" s="2">
         <v>384</v>
       </c>
@@ -27945,7 +27951,7 @@
       </c>
       <c r="S385" s="5"/>
     </row>
-    <row r="386" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A386" s="2">
         <v>385</v>
       </c>
@@ -28000,7 +28006,7 @@
       </c>
       <c r="S386" s="5"/>
     </row>
-    <row r="387" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A387" s="2">
         <v>386</v>
       </c>
@@ -28055,7 +28061,7 @@
       </c>
       <c r="S387" s="5"/>
     </row>
-    <row r="388" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A388" s="2">
         <v>387</v>
       </c>
@@ -28314,7 +28320,7 @@
       </c>
       <c r="S392" s="5"/>
     </row>
-    <row r="393" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A393" s="2">
         <v>392</v>
       </c>
@@ -28369,7 +28375,7 @@
       </c>
       <c r="S393" s="5"/>
     </row>
-    <row r="394" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A394" s="2">
         <v>393</v>
       </c>
@@ -29009,7 +29015,7 @@
       </c>
       <c r="S405" s="5"/>
     </row>
-    <row r="406" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A406" s="2">
         <v>405</v>
       </c>
@@ -29064,7 +29070,7 @@
       </c>
       <c r="S406" s="5"/>
     </row>
-    <row r="407" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A407" s="2">
         <v>406</v>
       </c>
@@ -29119,7 +29125,7 @@
       </c>
       <c r="S407" s="5"/>
     </row>
-    <row r="408" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A408" s="2">
         <v>407</v>
       </c>
@@ -29276,7 +29282,7 @@
       </c>
       <c r="S410" s="5"/>
     </row>
-    <row r="411" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A411" s="2">
         <v>410</v>
       </c>
@@ -29331,7 +29337,7 @@
       </c>
       <c r="S411" s="5"/>
     </row>
-    <row r="412" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A412" s="2">
         <v>411</v>
       </c>
@@ -29386,7 +29392,7 @@
       </c>
       <c r="S412" s="5"/>
     </row>
-    <row r="413" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="413" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A413" s="2">
         <v>412</v>
       </c>
@@ -29441,7 +29447,7 @@
       </c>
       <c r="S413" s="5"/>
     </row>
-    <row r="414" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="414" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A414" s="2">
         <v>413</v>
       </c>
@@ -29661,7 +29667,7 @@
       </c>
       <c r="S417" s="5"/>
     </row>
-    <row r="418" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="418" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A418" s="2">
         <v>417</v>
       </c>
@@ -29716,7 +29722,7 @@
       </c>
       <c r="S418" s="5"/>
     </row>
-    <row r="419" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="419" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A419" s="2">
         <v>418</v>
       </c>
@@ -29771,7 +29777,7 @@
       </c>
       <c r="S419" s="5"/>
     </row>
-    <row r="420" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="420" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A420" s="2">
         <v>419</v>
       </c>
@@ -29828,7 +29834,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="421" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="421" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A421" s="2">
         <v>420</v>
       </c>
@@ -29885,7 +29891,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="422" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="422" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A422" s="2">
         <v>421</v>
       </c>
@@ -30113,7 +30119,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="426" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="426" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A426" s="2">
         <v>425</v>
       </c>
@@ -30170,7 +30176,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="427" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="427" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A427" s="2">
         <v>426</v>
       </c>
@@ -30225,7 +30231,7 @@
       </c>
       <c r="S427" s="5"/>
     </row>
-    <row r="428" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="428" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A428" s="2">
         <v>427</v>
       </c>
@@ -30333,7 +30339,7 @@
       </c>
       <c r="S429" s="5"/>
     </row>
-    <row r="430" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="430" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A430" s="2">
         <v>429</v>
       </c>
@@ -30388,7 +30394,7 @@
       </c>
       <c r="S430" s="5"/>
     </row>
-    <row r="431" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="431" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A431" s="2">
         <v>430</v>
       </c>
@@ -30443,7 +30449,7 @@
       </c>
       <c r="S431" s="5"/>
     </row>
-    <row r="432" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="432" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A432" s="2">
         <v>431</v>
       </c>
@@ -30498,7 +30504,7 @@
       </c>
       <c r="S432" s="5"/>
     </row>
-    <row r="433" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="433" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A433" s="2">
         <v>432</v>
       </c>
@@ -30553,7 +30559,7 @@
       </c>
       <c r="S433" s="5"/>
     </row>
-    <row r="434" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="434" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A434" s="2">
         <v>433</v>
       </c>
@@ -30608,7 +30614,7 @@
       </c>
       <c r="S434" s="5"/>
     </row>
-    <row r="435" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="435" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A435" s="2">
         <v>434</v>
       </c>
@@ -30769,7 +30775,7 @@
       </c>
       <c r="S437" s="5"/>
     </row>
-    <row r="438" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="438" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A438" s="2">
         <v>437</v>
       </c>
@@ -31005,7 +31011,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="442" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="442" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A442" s="2">
         <v>441</v>
       </c>
@@ -31054,7 +31060,7 @@
       </c>
       <c r="S442" s="5"/>
     </row>
-    <row r="443" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="443" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A443" s="2">
         <v>442</v>
       </c>
@@ -31068,7 +31074,7 @@
         <v>137</v>
       </c>
       <c r="E443" s="3" t="s">
-        <v>21</v>
+        <v>1997</v>
       </c>
       <c r="F443" s="3" t="s">
         <v>323</v>
@@ -31219,7 +31225,7 @@
       </c>
       <c r="S445" s="5"/>
     </row>
-    <row r="446" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="446" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A446" s="2">
         <v>445</v>
       </c>
@@ -31274,7 +31280,7 @@
       </c>
       <c r="S446" s="5"/>
     </row>
-    <row r="447" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="447" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A447" s="2">
         <v>446</v>
       </c>
@@ -31329,7 +31335,7 @@
       </c>
       <c r="S447" s="5"/>
     </row>
-    <row r="448" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="448" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A448" s="2">
         <v>447</v>
       </c>
@@ -31384,7 +31390,7 @@
       </c>
       <c r="S448" s="5"/>
     </row>
-    <row r="449" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="449" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A449" s="2">
         <v>448</v>
       </c>
@@ -32103,7 +32109,7 @@
       </c>
       <c r="S461" s="5"/>
     </row>
-    <row r="462" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="462" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A462" s="2">
         <v>461</v>
       </c>
@@ -32158,7 +32164,7 @@
       </c>
       <c r="S462" s="5"/>
     </row>
-    <row r="463" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="463" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A463" s="2">
         <v>462</v>
       </c>
@@ -32323,7 +32329,7 @@
       </c>
       <c r="S465" s="5"/>
     </row>
-    <row r="466" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="466" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A466" s="2">
         <v>465</v>
       </c>
@@ -32378,7 +32384,7 @@
       </c>
       <c r="S466" s="5"/>
     </row>
-    <row r="467" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="467" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A467" s="2">
         <v>466</v>
       </c>
@@ -32433,7 +32439,7 @@
       </c>
       <c r="S467" s="5"/>
     </row>
-    <row r="468" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="468" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A468" s="2">
         <v>467</v>
       </c>
@@ -32763,7 +32769,7 @@
       </c>
       <c r="S473" s="5"/>
     </row>
-    <row r="474" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="474" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A474" s="2">
         <v>473</v>
       </c>
@@ -32818,7 +32824,7 @@
       </c>
       <c r="S474" s="5"/>
     </row>
-    <row r="475" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="475" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A475" s="2">
         <v>474</v>
       </c>
@@ -32983,7 +32989,7 @@
       </c>
       <c r="S477" s="5"/>
     </row>
-    <row r="478" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="478" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A478" s="2">
         <v>477</v>
       </c>
@@ -33038,7 +33044,7 @@
       </c>
       <c r="S478" s="5"/>
     </row>
-    <row r="479" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="479" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A479" s="2">
         <v>478</v>
       </c>
@@ -33093,7 +33099,7 @@
       </c>
       <c r="S479" s="5"/>
     </row>
-    <row r="480" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="480" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A480" s="2">
         <v>479</v>
       </c>
@@ -33478,7 +33484,7 @@
       </c>
       <c r="S486" s="5"/>
     </row>
-    <row r="487" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="487" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A487" s="2">
         <v>486</v>
       </c>
@@ -33533,7 +33539,7 @@
       </c>
       <c r="S487" s="5"/>
     </row>
-    <row r="488" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="488" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A488" s="2">
         <v>487</v>
       </c>
@@ -33643,7 +33649,7 @@
       </c>
       <c r="S489" s="5"/>
     </row>
-    <row r="490" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="490" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A490" s="2">
         <v>489</v>
       </c>
@@ -33808,7 +33814,7 @@
       </c>
       <c r="S492" s="5"/>
     </row>
-    <row r="493" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="493" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A493" s="2">
         <v>492</v>
       </c>
@@ -33863,7 +33869,7 @@
       </c>
       <c r="S493" s="5"/>
     </row>
-    <row r="494" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="494" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A494" s="2">
         <v>493</v>
       </c>
@@ -34028,7 +34034,7 @@
       </c>
       <c r="S496" s="5"/>
     </row>
-    <row r="497" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="497" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A497" s="2">
         <v>496</v>
       </c>
@@ -34472,7 +34478,7 @@
       </c>
       <c r="S504" s="5"/>
     </row>
-    <row r="505" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="505" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A505" s="2">
         <v>504</v>
       </c>
@@ -34798,7 +34804,7 @@
       </c>
       <c r="S510" s="5"/>
     </row>
-    <row r="511" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="511" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A511" s="2">
         <v>510</v>
       </c>
@@ -35014,7 +35020,7 @@
       </c>
       <c r="S514" s="5"/>
     </row>
-    <row r="515" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="515" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A515" s="2">
         <v>514</v>
       </c>
@@ -35069,7 +35075,7 @@
       </c>
       <c r="S515" s="5"/>
     </row>
-    <row r="516" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="516" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A516" s="2">
         <v>515</v>
       </c>
@@ -35548,7 +35554,7 @@
       </c>
       <c r="S524" s="5"/>
     </row>
-    <row r="525" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="525" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A525" s="2">
         <v>524</v>
       </c>
@@ -35603,7 +35609,7 @@
       </c>
       <c r="S525" s="5"/>
     </row>
-    <row r="526" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="526" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A526" s="2">
         <v>525</v>
       </c>
@@ -35878,7 +35884,7 @@
       </c>
       <c r="S530" s="5"/>
     </row>
-    <row r="531" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="531" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A531" s="2">
         <v>530</v>
       </c>
@@ -36204,7 +36210,7 @@
       </c>
       <c r="S536" s="5"/>
     </row>
-    <row r="537" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="537" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A537" s="2">
         <v>536</v>
       </c>
@@ -36259,7 +36265,7 @@
       </c>
       <c r="S537" s="5"/>
     </row>
-    <row r="538" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="538" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A538" s="2">
         <v>537</v>
       </c>
@@ -36314,7 +36320,7 @@
       </c>
       <c r="S538" s="5"/>
     </row>
-    <row r="539" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="539" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A539" s="2">
         <v>538</v>
       </c>
@@ -36589,7 +36595,7 @@
       </c>
       <c r="S543" s="5"/>
     </row>
-    <row r="544" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="544" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A544" s="2">
         <v>543</v>
       </c>
@@ -36644,7 +36650,7 @@
       </c>
       <c r="S544" s="5"/>
     </row>
-    <row r="545" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="545" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A545" s="2">
         <v>544</v>
       </c>
@@ -36699,7 +36705,7 @@
       </c>
       <c r="S545" s="5"/>
     </row>
-    <row r="546" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="546" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A546" s="2">
         <v>545</v>
       </c>
@@ -36750,7 +36756,7 @@
       </c>
       <c r="S546" s="5"/>
     </row>
-    <row r="547" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="547" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A547" s="2">
         <v>546</v>
       </c>
@@ -36911,7 +36917,7 @@
       </c>
       <c r="S549" s="5"/>
     </row>
-    <row r="550" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="550" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A550" s="2">
         <v>549</v>
       </c>
@@ -36966,7 +36972,7 @@
       </c>
       <c r="S550" s="5"/>
     </row>
-    <row r="551" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="551" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A551" s="2">
         <v>550</v>
       </c>
@@ -37021,7 +37027,7 @@
       </c>
       <c r="S551" s="5"/>
     </row>
-    <row r="552" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="552" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A552" s="2">
         <v>551</v>
       </c>
@@ -37076,7 +37082,7 @@
       </c>
       <c r="S552" s="5"/>
     </row>
-    <row r="553" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="553" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A553" s="2">
         <v>552</v>
       </c>
@@ -37398,7 +37404,7 @@
       </c>
       <c r="S558" s="5"/>
     </row>
-    <row r="559" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="559" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A559" s="2">
         <v>558</v>
       </c>
@@ -37453,7 +37459,7 @@
       </c>
       <c r="S559" s="5"/>
     </row>
-    <row r="560" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="560" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A560" s="2">
         <v>559</v>
       </c>
@@ -37508,7 +37514,7 @@
       </c>
       <c r="S560" s="5"/>
     </row>
-    <row r="561" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="561" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A561" s="2">
         <v>560</v>
       </c>
@@ -37783,7 +37789,7 @@
       </c>
       <c r="S565" s="5"/>
     </row>
-    <row r="566" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="566" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A566" s="2">
         <v>565</v>
       </c>
@@ -37838,7 +37844,7 @@
       </c>
       <c r="S566" s="5"/>
     </row>
-    <row r="567" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="567" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A567" s="2">
         <v>566</v>
       </c>
@@ -37893,7 +37899,7 @@
       </c>
       <c r="S567" s="5"/>
     </row>
-    <row r="568" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="568" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A568" s="2">
         <v>567</v>
       </c>
@@ -38168,7 +38174,7 @@
       </c>
       <c r="S572" s="5"/>
     </row>
-    <row r="573" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="573" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A573" s="2">
         <v>572</v>
       </c>
@@ -38223,7 +38229,7 @@
       </c>
       <c r="S573" s="5"/>
     </row>
-    <row r="574" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="574" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A574" s="2">
         <v>573</v>
       </c>
@@ -38553,7 +38559,7 @@
       </c>
       <c r="S579" s="5"/>
     </row>
-    <row r="580" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="580" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A580" s="2">
         <v>579</v>
       </c>
@@ -38608,7 +38614,7 @@
       </c>
       <c r="S580" s="5"/>
     </row>
-    <row r="581" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="581" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A581" s="2">
         <v>580</v>
       </c>
@@ -38663,7 +38669,7 @@
       </c>
       <c r="S581" s="5"/>
     </row>
-    <row r="582" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="582" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A582" s="2">
         <v>581</v>
       </c>
@@ -39087,7 +39093,7 @@
       </c>
       <c r="S589" s="5"/>
     </row>
-    <row r="590" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="590" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A590" s="2">
         <v>589</v>
       </c>
@@ -39142,7 +39148,7 @@
       </c>
       <c r="S590" s="5"/>
     </row>
-    <row r="591" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="591" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A591" s="2">
         <v>590</v>
       </c>
@@ -39307,7 +39313,7 @@
       </c>
       <c r="S593" s="5"/>
     </row>
-    <row r="594" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="594" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A594" s="2">
         <v>593</v>
       </c>
@@ -39574,7 +39580,7 @@
       </c>
       <c r="S598" s="5"/>
     </row>
-    <row r="599" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="599" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A599" s="2">
         <v>598</v>
       </c>
@@ -39629,7 +39635,7 @@
       </c>
       <c r="S599" s="5"/>
     </row>
-    <row r="600" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="600" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A600" s="2">
         <v>599</v>
       </c>
@@ -39682,7 +39688,7 @@
       </c>
       <c r="S600" s="5"/>
     </row>
-    <row r="601" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="601" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A601" s="2">
         <v>600</v>
       </c>
@@ -40002,7 +40008,7 @@
       </c>
       <c r="S606" s="5"/>
     </row>
-    <row r="607" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="607" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A607" s="2">
         <v>606</v>
       </c>
@@ -40214,7 +40220,7 @@
       </c>
       <c r="S610" s="5"/>
     </row>
-    <row r="611" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="611" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A611" s="2">
         <v>610</v>
       </c>
@@ -40626,7 +40632,7 @@
       </c>
       <c r="S618" s="5"/>
     </row>
-    <row r="619" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="619" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A619" s="2">
         <v>618</v>
       </c>
@@ -40980,7 +40986,7 @@
       <c r="S625" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:S1"/>
+  <autoFilter ref="A1:S625"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -47959,7 +47965,7 @@
       </c>
       <c r="D30" s="13"/>
     </row>
-    <row r="31" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="11">
         <v>31</v>
       </c>
@@ -47971,7 +47977,7 @@
       </c>
       <c r="D31" s="13"/>
     </row>
-    <row r="32" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="11">
         <v>32</v>
       </c>
@@ -48009,7 +48015,7 @@
       </c>
       <c r="D34" s="13"/>
     </row>
-    <row r="35" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="11">
         <v>35</v>
       </c>
@@ -48021,7 +48027,7 @@
       </c>
       <c r="D35" s="13"/>
     </row>
-    <row r="36" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="11">
         <v>36</v>
       </c>
@@ -48081,7 +48087,7 @@
       </c>
       <c r="D40" s="13"/>
     </row>
-    <row r="41" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="11">
         <v>41</v>
       </c>
@@ -48117,7 +48123,7 @@
       </c>
       <c r="D43" s="13"/>
     </row>
-    <row r="44" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" s="11">
         <v>44</v>
       </c>
@@ -48131,7 +48137,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="11">
         <v>45</v>
       </c>
@@ -48157,7 +48163,7 @@
       </c>
       <c r="D46" s="13"/>
     </row>
-    <row r="47" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="11">
         <v>47</v>
       </c>
@@ -48181,7 +48187,7 @@
       </c>
       <c r="D48" s="13"/>
     </row>
-    <row r="49" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="11">
         <v>49</v>
       </c>
@@ -48219,7 +48225,7 @@
       </c>
       <c r="D51" s="13"/>
     </row>
-    <row r="52" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="11">
         <v>52</v>
       </c>
@@ -48231,7 +48237,7 @@
       </c>
       <c r="D52" s="13"/>
     </row>
-    <row r="53" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="11">
         <v>53</v>
       </c>
@@ -48243,7 +48249,7 @@
       </c>
       <c r="D53" s="13"/>
     </row>
-    <row r="54" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="11">
         <v>54</v>
       </c>
@@ -48257,7 +48263,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="11">
         <v>55</v>
       </c>
@@ -48271,7 +48277,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="11">
         <v>56</v>
       </c>
@@ -48283,7 +48289,7 @@
       </c>
       <c r="D56" s="13"/>
     </row>
-    <row r="57" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="11">
         <v>57</v>
       </c>
@@ -48295,7 +48301,7 @@
       </c>
       <c r="D57" s="13"/>
     </row>
-    <row r="58" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="11">
         <v>58</v>
       </c>
@@ -48307,7 +48313,7 @@
       </c>
       <c r="D58" s="13"/>
     </row>
-    <row r="59" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="11">
         <v>59</v>
       </c>
@@ -48343,7 +48349,7 @@
       </c>
       <c r="D61" s="13"/>
     </row>
-    <row r="62" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="11">
         <v>62</v>
       </c>
@@ -48355,7 +48361,7 @@
       </c>
       <c r="D62" s="13"/>
     </row>
-    <row r="63" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="11">
         <v>63</v>
       </c>
@@ -48367,7 +48373,7 @@
       </c>
       <c r="D63" s="13"/>
     </row>
-    <row r="64" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="11">
         <v>64</v>
       </c>
@@ -48391,7 +48397,7 @@
       </c>
       <c r="D65" s="13"/>
     </row>
-    <row r="66" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="11">
         <v>66</v>
       </c>
@@ -48403,7 +48409,7 @@
       </c>
       <c r="D66" s="13"/>
     </row>
-    <row r="67" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="11">
         <v>67</v>
       </c>
@@ -48417,7 +48423,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="11">
         <v>68</v>
       </c>
@@ -48429,7 +48435,7 @@
       </c>
       <c r="D68" s="13"/>
     </row>
-    <row r="69" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="11">
         <v>69</v>
       </c>
@@ -48477,7 +48483,7 @@
       </c>
       <c r="D72" s="13"/>
     </row>
-    <row r="73" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="11">
         <v>73</v>
       </c>
@@ -48527,7 +48533,7 @@
       </c>
       <c r="D76" s="13"/>
     </row>
-    <row r="77" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="11">
         <v>77</v>
       </c>
@@ -48575,7 +48581,7 @@
       </c>
       <c r="D80" s="13"/>
     </row>
-    <row r="81" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="11">
         <v>81</v>
       </c>
@@ -48589,7 +48595,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="11">
         <v>82</v>
       </c>
@@ -48601,7 +48607,7 @@
       </c>
       <c r="D82" s="13"/>
     </row>
-    <row r="83" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="11">
         <v>83</v>
       </c>
@@ -48637,7 +48643,7 @@
       </c>
       <c r="D85" s="13"/>
     </row>
-    <row r="86" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="11">
         <v>86</v>
       </c>
@@ -48661,7 +48667,7 @@
       </c>
       <c r="D87" s="13"/>
     </row>
-    <row r="88" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="11">
         <v>88</v>
       </c>
@@ -48685,7 +48691,7 @@
       </c>
       <c r="D89" s="13"/>
     </row>
-    <row r="90" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="11">
         <v>90</v>
       </c>
@@ -48747,7 +48753,7 @@
       </c>
       <c r="D94" s="13"/>
     </row>
-    <row r="95" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="11">
         <v>95</v>
       </c>
@@ -48819,7 +48825,7 @@
       </c>
       <c r="D100" s="13"/>
     </row>
-    <row r="101" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="11">
         <v>101</v>
       </c>
@@ -48831,7 +48837,7 @@
       </c>
       <c r="D101" s="13"/>
     </row>
-    <row r="102" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="11">
         <v>102</v>
       </c>
@@ -48843,7 +48849,7 @@
       </c>
       <c r="D102" s="13"/>
     </row>
-    <row r="103" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A103" s="11">
         <v>103</v>
       </c>
@@ -48867,7 +48873,7 @@
       </c>
       <c r="D104" s="13"/>
     </row>
-    <row r="105" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="11">
         <v>105</v>
       </c>
@@ -48929,7 +48935,7 @@
       </c>
       <c r="D109" s="13"/>
     </row>
-    <row r="110" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" s="11">
         <v>110</v>
       </c>
@@ -48967,7 +48973,7 @@
       </c>
       <c r="D112" s="13"/>
     </row>
-    <row r="113" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" s="11">
         <v>113</v>
       </c>
@@ -49027,7 +49033,7 @@
       </c>
       <c r="D117" s="13"/>
     </row>
-    <row r="118" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" s="11">
         <v>118</v>
       </c>
@@ -49087,7 +49093,7 @@
       </c>
       <c r="D122" s="13"/>
     </row>
-    <row r="123" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" s="11">
         <v>123</v>
       </c>
@@ -49111,7 +49117,7 @@
       </c>
       <c r="D124" s="13"/>
     </row>
-    <row r="125" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" s="11">
         <v>126</v>
       </c>
@@ -49183,7 +49189,7 @@
       </c>
       <c r="D130" s="13"/>
     </row>
-    <row r="131" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" s="11">
         <v>132</v>
       </c>
@@ -49231,7 +49237,7 @@
       </c>
       <c r="D134" s="13"/>
     </row>
-    <row r="135" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" s="11">
         <v>136</v>
       </c>
@@ -49351,7 +49357,7 @@
       </c>
       <c r="D144" s="13"/>
     </row>
-    <row r="145" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" s="11">
         <v>146</v>
       </c>
@@ -49495,7 +49501,7 @@
       </c>
       <c r="D156" s="13"/>
     </row>
-    <row r="157" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A157" s="11">
         <v>158</v>
       </c>
@@ -49507,7 +49513,7 @@
       </c>
       <c r="D157" s="13"/>
     </row>
-    <row r="158" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" s="11">
         <v>159</v>
       </c>
@@ -49555,7 +49561,7 @@
       </c>
       <c r="D161" s="13"/>
     </row>
-    <row r="162" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162" s="11">
         <v>164</v>
       </c>
@@ -49677,7 +49683,7 @@
       </c>
       <c r="D171" s="13"/>
     </row>
-    <row r="172" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" s="11">
         <v>175</v>
       </c>
@@ -49725,7 +49731,7 @@
       </c>
       <c r="D175" s="13"/>
     </row>
-    <row r="176" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176" s="11">
         <v>179</v>
       </c>
@@ -49785,7 +49791,7 @@
       </c>
       <c r="D180" s="13"/>
     </row>
-    <row r="181" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A181" s="11">
         <v>184</v>
       </c>
@@ -49809,7 +49815,7 @@
       </c>
       <c r="D182" s="13"/>
     </row>
-    <row r="183" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183" s="11">
         <v>186</v>
       </c>
@@ -49821,7 +49827,7 @@
       </c>
       <c r="D183" s="13"/>
     </row>
-    <row r="184" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A184" s="11">
         <v>187</v>
       </c>
@@ -49845,7 +49851,7 @@
       </c>
       <c r="D185" s="13"/>
     </row>
-    <row r="186" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186" s="11">
         <v>189</v>
       </c>
@@ -49857,7 +49863,7 @@
       </c>
       <c r="D186" s="13"/>
     </row>
-    <row r="187" spans="1:4" ht="144" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A187" s="11">
         <v>190</v>
       </c>
@@ -49893,7 +49899,7 @@
       </c>
       <c r="D189" s="13"/>
     </row>
-    <row r="190" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190" s="11">
         <v>193</v>
       </c>
@@ -49919,7 +49925,7 @@
       </c>
       <c r="D191" s="13"/>
     </row>
-    <row r="192" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192" s="11">
         <v>195</v>
       </c>
@@ -50015,7 +50021,7 @@
       </c>
       <c r="D199" s="13"/>
     </row>
-    <row r="200" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A200" s="11">
         <v>203</v>
       </c>
@@ -50039,7 +50045,7 @@
       </c>
       <c r="D201" s="13"/>
     </row>
-    <row r="202" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A202" s="11">
         <v>205</v>
       </c>
@@ -50065,7 +50071,7 @@
       </c>
       <c r="D203" s="13"/>
     </row>
-    <row r="204" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A204" s="11">
         <v>207</v>
       </c>
@@ -50103,7 +50109,7 @@
       </c>
       <c r="D206" s="13"/>
     </row>
-    <row r="207" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A207" s="11">
         <v>210</v>
       </c>
@@ -50129,7 +50135,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="209" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A209" s="11">
         <v>212</v>
       </c>
@@ -50153,7 +50159,7 @@
       </c>
       <c r="D210" s="13"/>
     </row>
-    <row r="211" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A211" s="11">
         <v>215</v>
       </c>
@@ -50165,7 +50171,7 @@
       </c>
       <c r="D211" s="13"/>
     </row>
-    <row r="212" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A212" s="11">
         <v>216</v>
       </c>
@@ -50191,7 +50197,7 @@
       </c>
       <c r="D213" s="13"/>
     </row>
-    <row r="214" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A214" s="11">
         <v>218</v>
       </c>
@@ -50215,7 +50221,7 @@
       </c>
       <c r="D215" s="13"/>
     </row>
-    <row r="216" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A216" s="11">
         <v>220</v>
       </c>
@@ -50229,7 +50235,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="217" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A217" s="11">
         <v>221</v>
       </c>
@@ -50243,7 +50249,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="218" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A218" s="11">
         <v>222</v>
       </c>
@@ -50257,7 +50263,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="219" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A219" s="11">
         <v>223</v>
       </c>
@@ -50271,7 +50277,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="220" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A220" s="11">
         <v>224</v>
       </c>

</xml_diff>